<commit_message>
Update project with latest changes
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.195.129</t>
+          <t>192.168.40.89</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -471,12 +471,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>192.168.78.193</t>
+          <t>192.168.37.146</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.108.95</t>
+          <t>192.168.191.110</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -501,12 +501,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.188.66</t>
+          <t>192.168.160.158</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>192.168.58.149</t>
+          <t>192.168.139.158</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -531,12 +531,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>192.168.82.253</t>
+          <t>192.168.194.31</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -546,12 +546,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>192.168.143.218</t>
+          <t>192.168.161.218</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -561,12 +561,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>192.168.42.208</t>
+          <t>192.168.0.46</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -576,12 +576,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>192.168.37.148</t>
+          <t>192.168.246.89</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -591,7 +591,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>192.168.134.39</t>
+          <t>192.168.155.56</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -606,12 +606,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>192.168.190.200</t>
+          <t>192.168.254.143</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -621,12 +621,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>192.168.68.119</t>
+          <t>192.168.54.92</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -636,12 +636,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>192.168.68.44</t>
+          <t>192.168.154.221</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>192.168.17.188</t>
+          <t>192.168.228.99</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>192.168.35.51</t>
+          <t>192.168.203.93</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>192.168.51.229</t>
+          <t>192.168.30.143</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -696,12 +696,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>192.168.226.241</t>
+          <t>192.168.201.222</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>192.168.56.231</t>
+          <t>192.168.124.244</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -726,12 +726,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>192.168.145.67</t>
+          <t>192.168.240.180</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -741,12 +741,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>192.168.98.243</t>
+          <t>192.168.104.18</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -756,12 +756,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>192.168.199.247</t>
+          <t>192.168.33.37</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -771,12 +771,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>192.168.100.17</t>
+          <t>192.168.143.111</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>192.168.136.234</t>
+          <t>192.168.128.159</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -801,12 +801,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>192.168.161.230</t>
+          <t>192.168.204.48</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -816,12 +816,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>192.168.227.108</t>
+          <t>192.168.89.247</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -831,12 +831,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>192.168.16.54</t>
+          <t>192.168.196.176</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -846,12 +846,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>192.168.221.165</t>
+          <t>192.168.74.30</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>192.168.67.118</t>
+          <t>192.168.124.82</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>192.168.165.202</t>
+          <t>192.168.85.206</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -891,12 +891,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>192.168.12.130</t>
+          <t>192.168.48.54</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>192.168.25.22</t>
+          <t>192.168.20.74</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -921,12 +921,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>192.168.228.102</t>
+          <t>192.168.221.8</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -936,12 +936,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>192.168.190.85</t>
+          <t>192.168.118.28</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -951,12 +951,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>192.168.178.134</t>
+          <t>192.168.145.160</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -966,12 +966,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>192.168.195.42</t>
+          <t>192.168.242.174</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>192.168.71.66</t>
+          <t>192.168.20.105</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -996,12 +996,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>192.168.57.109</t>
+          <t>192.168.197.12</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1011,12 +1011,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>192.168.146.104</t>
+          <t>192.168.80.97</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1026,12 +1026,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>192.168.239.66</t>
+          <t>192.168.147.178</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>192.168.17.4</t>
+          <t>192.168.3.218</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1056,12 +1056,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>192.168.219.119</t>
+          <t>192.168.176.112</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1071,12 +1071,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>192.168.160.140</t>
+          <t>192.168.110.127</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>192.168.186.51</t>
+          <t>192.168.87.54</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1101,12 +1101,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>192.168.252.77</t>
+          <t>192.168.59.121</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1116,12 +1116,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>192.168.126.12</t>
+          <t>192.168.98.230</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1131,12 +1131,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>192.168.136.198</t>
+          <t>192.168.115.112</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>192.168.206.74</t>
+          <t>192.168.202.83</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>192.168.105.56</t>
+          <t>192.168.247.218</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1176,12 +1176,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>192.168.0.99</t>
+          <t>192.168.233.61</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1191,12 +1191,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>192.168.161.100</t>
+          <t>192.168.30.79</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>192.168.73.119</t>
+          <t>192.168.141.60</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1221,12 +1221,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>192.168.46.94</t>
+          <t>192.168.104.157</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1236,12 +1236,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>192.168.85.240</t>
+          <t>192.168.70.170</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1251,12 +1251,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>192.168.146.129</t>
+          <t>192.168.134.123</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1266,12 +1266,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>192.168.149.190</t>
+          <t>192.168.166.66</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>192.168.209.251</t>
+          <t>192.168.210.97</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1296,12 +1296,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>192.168.77.206</t>
+          <t>192.168.69.177</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>192.168.77.25</t>
+          <t>192.168.144.108</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1326,12 +1326,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>192.168.131.255</t>
+          <t>192.168.232.187</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>192.168.117.102</t>
+          <t>192.168.98.115</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1356,12 +1356,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>192.168.192.82</t>
+          <t>192.168.21.150</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1371,12 +1371,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>192.168.40.102</t>
+          <t>192.168.225.75</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1386,12 +1386,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>192.168.169.150</t>
+          <t>192.168.89.127</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>192.168.164.204</t>
+          <t>192.168.59.153</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1416,12 +1416,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>192.168.151.131</t>
+          <t>192.168.197.55</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>192.168.138.212</t>
+          <t>192.168.39.116</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1446,12 +1446,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>192.168.50.77</t>
+          <t>192.168.151.41</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1461,12 +1461,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>192.168.250.250</t>
+          <t>192.168.162.42</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1476,12 +1476,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>192.168.232.3</t>
+          <t>192.168.171.112</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1491,12 +1491,12 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>192.168.216.239</t>
+          <t>192.168.189.254</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1506,12 +1506,12 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>192.168.89.112</t>
+          <t>192.168.218.19</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>192.168.236.70</t>
+          <t>192.168.36.161</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>192.168.104.198</t>
+          <t>192.168.196.89</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1551,12 +1551,12 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>192.168.249.251</t>
+          <t>192.168.59.150</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1566,12 +1566,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>192.168.137.22</t>
+          <t>192.168.170.22</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1581,12 +1581,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>192.168.231.185</t>
+          <t>192.168.189.84</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>192.168.127.89</t>
+          <t>192.168.120.35</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -1611,12 +1611,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>192.168.218.198</t>
+          <t>192.168.198.141</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1626,12 +1626,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>192.168.206.247</t>
+          <t>192.168.119.200</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1641,12 +1641,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>192.168.127.130</t>
+          <t>192.168.137.189</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1656,12 +1656,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>192.168.248.127</t>
+          <t>192.168.240.39</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1671,12 +1671,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>192.168.141.126</t>
+          <t>192.168.254.132</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>192.168.158.185</t>
+          <t>192.168.208.45</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -1701,12 +1701,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>192.168.173.254</t>
+          <t>192.168.118.16</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>192.168.58.103</t>
+          <t>192.168.163.165</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>192.168.222.69</t>
+          <t>192.168.216.174</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -1746,12 +1746,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>192.168.112.45</t>
+          <t>192.168.153.179</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1761,12 +1761,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>192.168.200.108</t>
+          <t>192.168.71.16</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1776,12 +1776,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>192.168.144.109</t>
+          <t>192.168.242.151</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1791,12 +1791,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>192.168.209.100</t>
+          <t>192.168.182.40</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>192.168.99.126</t>
+          <t>192.168.54.108</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -1821,12 +1821,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>192.168.90.21</t>
+          <t>192.168.67.227</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1836,12 +1836,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>192.168.168.172</t>
+          <t>192.168.209.6</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1851,12 +1851,12 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>192.168.127.136</t>
+          <t>192.168.175.190</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -1866,12 +1866,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>192.168.70.101</t>
+          <t>192.168.247.183</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1881,12 +1881,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>192.168.125.88</t>
+          <t>192.168.95.193</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>192.168.252.185</t>
+          <t>192.168.35.182</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -1911,12 +1911,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>192.168.6.9</t>
+          <t>192.168.206.44</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1926,12 +1926,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>192.168.149.99</t>
+          <t>192.168.53.161</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -1941,12 +1941,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>192.168.48.201</t>
+          <t>192.168.248.190</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -1956,12 +1956,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>192.168.11.35</t>
+          <t>192.168.138.204</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>192.168.84.248</t>
+          <t>192.168.85.8</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>192.168.25.167</t>
+          <t>192.168.145.244</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2001,12 +2001,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>192.168.226.218</t>
+          <t>192.168.179.235</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2016,12 +2016,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>192.168.218.151</t>
+          <t>192.168.86.173</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2031,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>192.168.16.144</t>
+          <t>192.168.230.194</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2046,12 +2046,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>192.168.231.124</t>
+          <t>192.168.75.58</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2061,12 +2061,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>192.168.67.182</t>
+          <t>192.168.107.44</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -2076,12 +2076,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>192.168.79.194</t>
+          <t>192.168.30.137</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -2091,12 +2091,12 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>192.168.116.43</t>
+          <t>192.168.226.101</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2106,12 +2106,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>192.168.242.251</t>
+          <t>192.168.17.103</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2121,12 +2121,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>192.168.71.42</t>
+          <t>192.168.76.34</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2136,12 +2136,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>192.168.6.93</t>
+          <t>192.168.30.17</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2151,12 +2151,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>192.168.253.42</t>
+          <t>192.168.196.20</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2166,12 +2166,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>192.168.70.145</t>
+          <t>192.168.71.184</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2181,12 +2181,12 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>192.168.75.61</t>
+          <t>192.168.175.100</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2196,12 +2196,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>192.168.54.220</t>
+          <t>192.168.43.172</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2211,12 +2211,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>192.168.93.178</t>
+          <t>192.168.180.99</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2226,12 +2226,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>192.168.149.255</t>
+          <t>192.168.148.167</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2241,12 +2241,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>192.168.85.60</t>
+          <t>192.168.116.206</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2256,12 +2256,12 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>192.168.92.186</t>
+          <t>192.168.135.35</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2271,12 +2271,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>192.168.236.222</t>
+          <t>192.168.128.181</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2286,12 +2286,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>192.168.168.157</t>
+          <t>192.168.218.92</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2301,12 +2301,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>192.168.234.83</t>
+          <t>192.168.61.232</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2316,12 +2316,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>192.168.203.3</t>
+          <t>192.168.205.195</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2331,12 +2331,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>192.168.206.217</t>
+          <t>192.168.161.134</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2346,12 +2346,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>192.168.82.126</t>
+          <t>192.168.180.40</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>192.168.83.104</t>
+          <t>192.168.252.180</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -2376,12 +2376,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>192.168.11.123</t>
+          <t>192.168.118.72</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2391,12 +2391,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>192.168.137.31</t>
+          <t>192.168.197.69</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2406,12 +2406,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>192.168.214.109</t>
+          <t>192.168.129.177</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2421,12 +2421,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>192.168.136.99</t>
+          <t>192.168.172.212</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2436,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>192.168.29.184</t>
+          <t>192.168.136.214</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2451,12 +2451,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>192.168.166.179</t>
+          <t>192.168.145.168</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2466,12 +2466,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>192.168.173.223</t>
+          <t>192.168.99.20</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>192.168.19.8</t>
+          <t>192.168.109.15</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -2496,12 +2496,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>192.168.72.69</t>
+          <t>192.168.207.211</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option5</t>
         </is>
       </c>
     </row>
@@ -2511,12 +2511,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>192.168.206.173</t>
+          <t>192.168.252.77</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2526,12 +2526,12 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>192.168.5.33</t>
+          <t>192.168.180.114</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -2541,12 +2541,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>192.168.143.137</t>
+          <t>192.168.78.161</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>option5</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -2556,12 +2556,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>192.168.18.4</t>
+          <t>192.168.253.225</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2571,12 +2571,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>192.168.92.36</t>
+          <t>192.168.118.134</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2586,12 +2586,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>192.168.33.6</t>
+          <t>192.168.171.32</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option3</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>192.168.125.239</t>
+          <t>192.168.108.207</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>192.168.161.120</t>
+          <t>192.168.83.72</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -2631,12 +2631,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>192.168.177.157</t>
+          <t>192.168.86.185</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>option1</t>
+          <t>option2</t>
         </is>
       </c>
     </row>
@@ -2646,12 +2646,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>192.168.89.184</t>
+          <t>192.168.190.243</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>option3</t>
+          <t>option4</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>192.168.216.80</t>
+          <t>192.168.188.83</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -2676,12 +2676,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>192.168.35.219</t>
+          <t>192.168.118.69</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>option2</t>
+          <t>option1</t>
         </is>
       </c>
     </row>
@@ -2691,12 +2691,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>192.168.169.215</t>
+          <t>192.168.120.101</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>option4</t>
+          <t>option3</t>
         </is>
       </c>
     </row>

</xml_diff>